<commit_message>
Ran flux processing data
</commit_message>
<xml_diff>
--- a/GC-Data-Raw-R/n2o_analysis_draft.xlsx
+++ b/GC-Data-Raw-R/n2o_analysis_draft.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="2420" windowWidth="16240" windowHeight="16740" tabRatio="850" activeTab="1"/>
+    <workbookView xWindow="200" yWindow="2420" windowWidth="16240" windowHeight="16740" tabRatio="850" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Vial info" sheetId="1" r:id="rId1"/>
@@ -501,8 +501,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="167">
+  <cellStyleXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -676,7 +678,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="167">
+  <cellStyles count="169">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -760,6 +762,7 @@
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -843,6 +846,7 @@
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1254,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:K1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1310,8 +1314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>